<commit_message>
Battle System -by event
</commit_message>
<xml_diff>
--- a/Practice_3/Assets/Resources/PlayerStat.xlsx
+++ b/Practice_3/Assets/Resources/PlayerStat.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PSK\Desktop\Unity_Programming_Practice_3\Practice_3\Assets\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FC7840F1-EB06-4C53-B445-B7EEFF3BBE9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31F43B3B-562F-4BEA-A055-B50525114BB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{FB721D61-A7C3-4471-9F32-6A2F5D243075}"/>
   </bookViews>
@@ -433,7 +433,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -454,7 +454,7 @@
         <v>3</v>
       </c>
       <c r="B2">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C2">
         <v>3</v>
@@ -465,7 +465,7 @@
         <v>4</v>
       </c>
       <c r="B3">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C3">
         <v>2</v>
@@ -476,7 +476,7 @@
         <v>5</v>
       </c>
       <c r="B4">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="C4">
         <v>5</v>
@@ -487,7 +487,7 @@
         <v>6</v>
       </c>
       <c r="B5">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -498,10 +498,10 @@
         <v>7</v>
       </c>
       <c r="B6">
-        <v>6</v>
+        <v>100</v>
       </c>
       <c r="C6">
-        <v>6</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>